<commit_message>
commit : aws 업로드 전 확인
</commit_message>
<xml_diff>
--- a/1.개발스케줄표/개발스케줄표.xlsx
+++ b/1.개발스케줄표/개발스케줄표.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\devSpace\ToyProjects\JAVA\RealTimeChatProgram\1.개발스케줄표\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\devSpace\SpringProjects\ChatProgram\ChatProgram\1.개발스케줄표\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9522190-3CD2-4C62-B2E8-8553E37C5362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4241C7-D278-444A-8129-10D07DC68EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1755" windowWidth="18585" windowHeight="11295" xr2:uid="{CDC8B9AB-2BEB-4A41-AD0A-1014A8107960}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CDC8B9AB-2BEB-4A41-AD0A-1014A8107960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -540,16 +540,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -559,24 +577,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -896,7 +896,7 @@
   <dimension ref="B3:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:G9"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -911,13 +911,13 @@
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="3" t="s">
         <v>4</v>
       </c>
@@ -929,16 +929,16 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="C5" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="5">
         <v>45468</v>
       </c>
@@ -950,14 +950,14 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="9">
         <v>45468</v>
       </c>
@@ -969,14 +969,14 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="20"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="11">
         <v>45468</v>
       </c>
@@ -988,99 +988,99 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
       <c r="H8" s="13">
         <v>45468</v>
       </c>
       <c r="I8" s="13">
-        <v>45468</v>
+        <v>45470</v>
       </c>
       <c r="J8" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="23"/>
-      <c r="C9" s="24" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="10">
-        <v>45468</v>
+        <v>45470</v>
       </c>
       <c r="I9" s="10">
-        <v>45468</v>
+        <v>45470</v>
       </c>
       <c r="J9" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
       <c r="H10" s="5">
-        <v>45469</v>
+        <v>45471</v>
       </c>
       <c r="I10" s="5">
-        <v>45469</v>
+        <v>45471</v>
       </c>
       <c r="J10" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="19"/>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="5">
-        <v>45469</v>
+        <v>45471</v>
       </c>
       <c r="I11" s="5">
-        <v>45469</v>
+        <v>45471</v>
       </c>
       <c r="J11" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="19"/>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="5">
-        <v>45469</v>
+        <v>45472</v>
       </c>
       <c r="I12" s="5">
-        <v>45469</v>
+        <v>45472</v>
       </c>
       <c r="J12" s="7">
         <v>1</v>
@@ -1090,187 +1090,184 @@
       <c r="B13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
       <c r="H13" s="13">
-        <v>45470</v>
+        <v>45473</v>
       </c>
       <c r="I13" s="13">
-        <v>45470</v>
+        <v>45473</v>
       </c>
       <c r="J13" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="18" t="s">
+    <row r="14" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
       <c r="H14" s="5">
-        <v>45470</v>
+        <v>45473</v>
       </c>
       <c r="I14" s="5">
-        <v>45470</v>
+        <v>45473</v>
       </c>
       <c r="J14" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="19"/>
-      <c r="C15" s="17" t="s">
+    <row r="15" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="18"/>
+      <c r="C15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="9">
-        <v>45470</v>
-      </c>
-      <c r="I15" s="9">
-        <v>45470</v>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="5">
+        <v>45473</v>
+      </c>
+      <c r="I15" s="5">
+        <v>45473</v>
       </c>
       <c r="J15" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="19"/>
-      <c r="C16" s="17" t="s">
+    <row r="16" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="18"/>
+      <c r="C16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="9">
-        <v>45470</v>
-      </c>
-      <c r="I16" s="9">
-        <v>45470</v>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="5">
+        <v>45473</v>
+      </c>
+      <c r="I16" s="5">
+        <v>45473</v>
       </c>
       <c r="J16" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="19"/>
-      <c r="C17" s="17" t="s">
+    <row r="17" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="18"/>
+      <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="9">
-        <v>45470</v>
-      </c>
-      <c r="I17" s="9">
-        <v>45470</v>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="5">
+        <v>45474</v>
+      </c>
+      <c r="I17" s="5">
+        <v>45474</v>
       </c>
       <c r="J17" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="19"/>
-      <c r="C18" s="17" t="s">
+      <c r="B18" s="18"/>
+      <c r="C18" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="9">
-        <v>45471</v>
-      </c>
-      <c r="I18" s="9">
-        <v>45471</v>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="5">
+        <v>45474</v>
+      </c>
+      <c r="I18" s="5">
+        <v>45474</v>
       </c>
       <c r="J18" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="19"/>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="9">
-        <v>45471</v>
+        <v>45475</v>
       </c>
       <c r="I19" s="9">
-        <v>45471</v>
+        <v>45475</v>
       </c>
       <c r="J19" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="19"/>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="18"/>
+      <c r="C20" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="9">
-        <v>45472</v>
+        <v>45476</v>
       </c>
       <c r="I20" s="9">
-        <v>45472</v>
+        <v>45476</v>
       </c>
       <c r="J20" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="23"/>
-      <c r="C21" s="28" t="s">
+      <c r="B21" s="19"/>
+      <c r="C21" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
       <c r="H21" s="10">
-        <v>45472</v>
+        <v>45477</v>
       </c>
       <c r="I21" s="10">
-        <v>45472</v>
+        <v>45479</v>
       </c>
       <c r="J21" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C4:G4"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -1280,11 +1277,14 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C15:G15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>